<commit_message>
add parsePdf and genExcel parameters
</commit_message>
<xml_diff>
--- a/data/quiz.xlsx
+++ b/data/quiz.xlsx
@@ -11,12 +11,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>question</t>
+    <t>question1</t>
   </si>
   <si>
-    <t>answer</t>
+    <t>amswer1</t>
+  </si>
+  <si>
+    <t>question2</t>
+  </si>
+  <si>
+    <t>amswer2</t>
   </si>
 </sst>
 </file>
@@ -62,7 +68,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -76,6 +82,22 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>